<commit_message>
neue sensor excel file
</commit_message>
<xml_diff>
--- a/Sharp_IR-Sensor_150cm.xlsx
+++ b/Sharp_IR-Sensor_150cm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyuce\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5754F09B-2F73-4B6E-A628-4E32CAB13EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F16664-C056-4164-9EB9-F8239CE1ABF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{3FAD9BF2-B5AE-4568-AE41-C64B5EC617C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{3FAD9BF2-B5AE-4568-AE41-C64B5EC617C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Front" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1082,9 +1082,6 @@
                 <c:pt idx="6">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1095,25 +1092,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1380,25 +1377,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1485,25 +1482,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1515,25 +1512,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>7.447725503281058E-2</c:v>
+                  <c:v>7.0103488581749446E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.145812479145812E-2</c:v>
+                  <c:v>4.3873842786886261E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0162106550995434E-2</c:v>
+                  <c:v>2.9534969752361053E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3210710710710708E-2</c:v>
+                  <c:v>2.3589583372192066E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.8518518518518517E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5911745078411744E-2</c:v>
+                  <c:v>1.6595011160228549E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3304971638304972E-2</c:v>
+                  <c:v>1.5720689633733111E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1840,9 +1837,6 @@
                 <c:pt idx="6">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1856,22 +1850,22 @@
                   <c:v>440</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,22 +2135,22 @@
                   <c:v>440</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2246,22 +2240,22 @@
                   <c:v>440</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2273,25 +2267,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>7.447725503281058E-2</c:v>
+                  <c:v>6.6055809908268912E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.145812479145812E-2</c:v>
+                  <c:v>4.2364085396872281E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0162106550995434E-2</c:v>
+                  <c:v>2.8210587636817143E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3210710710710708E-2</c:v>
+                  <c:v>2.3133789527232149E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.8518518518518517E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5911745078411744E-2</c:v>
+                  <c:v>1.5595513546333217E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3304971638304972E-2</c:v>
+                  <c:v>1.4210932243719127E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5824,14 +5818,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>442052</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:colOff>489677</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>7666</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>283029</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:colOff>330654</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6377,17 +6371,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFDD5582-8EC9-4773-B372-BA84A49938AD}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6404,7 +6398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -6416,7 +6410,7 @@
         <v>2.0366598778004071E-3</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D13" si="0">1/(A2+$D$22)</f>
+        <f t="shared" ref="D2:D20" si="0">1/(A2+$D$22)</f>
         <v>3.5714285714285712E-2</v>
       </c>
       <c r="E2">
@@ -6424,7 +6418,7 @@
         <v>3.2844639232569257E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>30</v>
       </c>
@@ -6432,7 +6426,7 @@
         <v>390</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C13" si="1">1/B3</f>
+        <f t="shared" ref="C3:C20" si="1">1/B3</f>
         <v>2.5641025641025641E-3</v>
       </c>
       <c r="D3">
@@ -6440,11 +6434,11 @@
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E13" si="2">$D$23*B3+$D$24</f>
+        <f t="shared" ref="E3:E20" si="2">$D$23*B3+$D$24</f>
         <v>2.6315789473684206E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>40</v>
       </c>
@@ -6464,7 +6458,7 @@
         <v>2.0045508022081729E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>50</v>
       </c>
@@ -6484,7 +6478,7 @@
         <v>1.7589109102897255E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>60</v>
       </c>
@@ -6504,7 +6498,7 @@
         <v>1.4421647338685697E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>70</v>
       </c>
@@ -6524,7 +6518,7 @@
         <v>1.2547027110887017E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>80</v>
       </c>
@@ -6544,7 +6538,7 @@
         <v>1.1124901420832847E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>90</v>
       </c>
@@ -6564,7 +6558,7 @@
         <v>1.0155270268523187E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>100</v>
       </c>
@@ -6584,7 +6578,7 @@
         <v>9.1856391162135238E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>110</v>
       </c>
@@ -6604,7 +6598,7 @@
         <v>8.2806500407245076E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>120</v>
       </c>
@@ -6624,7 +6618,7 @@
         <v>7.698871349338712E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>130</v>
       </c>
@@ -6644,42 +6638,47 @@
         <v>7.246376811594203E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>140</v>
       </c>
+      <c r="B14">
+        <v>82</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>1.2195121951219513E-2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>6.7567567567567571E-3</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>6.4060298129258297E-3</v>
+      </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>150</v>
       </c>
+      <c r="B15">
+        <v>79</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>1.2658227848101266E-2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>6.3291139240506328E-3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>6.2121035824638975E-3</v>
+      </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>4</v>
       </c>
@@ -6687,7 +6686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>6</v>
       </c>
@@ -6696,7 +6695,7 @@
         <v>6.464207682064408E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>5</v>
       </c>
@@ -6705,7 +6704,7 @@
         <v>1.1053795136330155E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>8</v>
       </c>
@@ -6714,7 +6713,7 @@
         <v>15469.800000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>9</v>
       </c>
@@ -6733,17 +6732,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F45B06-3885-459E-8A3A-CD8D9697C8CC}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6760,36 +6759,36 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="C2">
         <f>1/B2</f>
-        <v>2.2727272727272726E-3</v>
+        <v>2.352941176470588E-3</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D8" si="0">1/(A2+$D$12)</f>
+        <f t="shared" ref="D2:D9" si="0">1/(A2+$D$12)</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E8" si="1">$D$13*B2+$D$14</f>
-        <v>7.447725503281058E-2</v>
+        <f t="shared" ref="E2:E9" si="1">$D$13*B2+$D$14</f>
+        <v>7.0103488581749446E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20</v>
       </c>
       <c r="B3">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" si="2">1/B3</f>
-        <v>4.0000000000000001E-3</v>
+        <f t="shared" ref="C3:C9" si="2">1/B3</f>
+        <v>3.6363636363636364E-3</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
@@ -6797,19 +6796,19 @@
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
-        <v>4.145812479145812E-2</v>
+        <v>4.3873842786886261E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
       <c r="B4">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C4">
         <f t="shared" si="2"/>
-        <v>5.4054054054054057E-3</v>
+        <v>5.1813471502590676E-3</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -6817,19 +6816,19 @@
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>3.0162106550995434E-2</v>
+        <v>2.9534969752361053E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40</v>
       </c>
       <c r="B5">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="C5">
         <f t="shared" si="2"/>
-        <v>6.8965517241379309E-3</v>
+        <v>6.2893081761006293E-3</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -6837,19 +6836,19 @@
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>2.3210710710710708E-2</v>
+        <v>2.3589583372192066E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>50</v>
       </c>
       <c r="B6">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C6">
         <f t="shared" si="2"/>
-        <v>8.4745762711864406E-3</v>
+        <v>7.6923076923076927E-3</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -6860,16 +6859,16 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
-        <v>9.7087378640776691E-3</v>
+        <v>8.4033613445378148E-3</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -6877,19 +6876,19 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>1.5911745078411744E-2</v>
+        <v>1.6595011160228549E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>70</v>
       </c>
       <c r="B8">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
-        <v>1.1363636363636364E-2</v>
+        <v>8.771929824561403E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -6897,15 +6896,10 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>1.3304971638304972E-2</v>
+        <v>1.5720689633733111E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>4</v>
       </c>
@@ -6913,40 +6907,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13">
         <f>(D3-D8)/(B3-B8)</f>
-        <v>1.7378489600711821E-4</v>
+        <v>1.748643052990879E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14">
         <f>D6-(D13*B6)</f>
-        <v>-1.9880992103214305E-3</v>
+        <v>-4.2138411703629107E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15">
         <f>1/D13</f>
-        <v>5754.2400000000007</v>
+        <v>5718.72</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16">
         <f>D14/D13</f>
-        <v>-11.439999999999991</v>
+        <v>-24.097777777777786</v>
       </c>
     </row>
   </sheetData>
@@ -6960,16 +6954,16 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6986,7 +6980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -6998,24 +6992,24 @@
         <v>2.2727272727272726E-3</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D8" si="0">1/(A2+$D$12)</f>
+        <f t="shared" ref="D2:D9" si="0">1/(A2+$D$12)</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E8" si="1">$D$13*B2+$D$14</f>
-        <v>7.447725503281058E-2</v>
+        <f t="shared" ref="E2:E9" si="1">$D$13*B2+$D$14</f>
+        <v>6.6055809908268912E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20</v>
       </c>
       <c r="B3">
-        <v>250</v>
+        <v>286</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" si="2">1/B3</f>
-        <v>4.0000000000000001E-3</v>
+        <f t="shared" ref="C3:C9" si="2">1/B3</f>
+        <v>3.4965034965034965E-3</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
@@ -7023,19 +7017,19 @@
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
-        <v>4.145812479145812E-2</v>
+        <v>4.2364085396872281E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
       <c r="B4">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="C4">
         <f t="shared" si="2"/>
-        <v>5.4054054054054057E-3</v>
+        <v>5.1546391752577319E-3</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -7043,19 +7037,19 @@
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>3.0162106550995434E-2</v>
+        <v>2.8210587636817143E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40</v>
       </c>
       <c r="B5">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="C5">
         <f t="shared" si="2"/>
-        <v>6.8965517241379309E-3</v>
+        <v>6.2111801242236021E-3</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -7063,19 +7057,19 @@
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>2.3210710710710708E-2</v>
+        <v>2.3133789527232149E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>50</v>
       </c>
       <c r="B6">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C6">
         <f t="shared" si="2"/>
-        <v>8.4745762711864406E-3</v>
+        <v>7.6335877862595417E-3</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -7086,16 +7080,16 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
-        <v>9.7087378640776691E-3</v>
+        <v>8.9285714285714281E-3</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -7103,19 +7097,19 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>1.5911745078411744E-2</v>
+        <v>1.5595513546333217E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>70</v>
       </c>
       <c r="B8">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
-        <v>1.1363636363636364E-2</v>
+        <v>9.7087378640776691E-3</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -7123,15 +7117,10 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>1.3304971638304972E-2</v>
+        <v>1.4210932243719127E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>4</v>
       </c>
@@ -7139,40 +7128,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13">
         <f>(D3-D8)/(B3-B8)</f>
-        <v>1.7378489600711821E-4</v>
+        <v>1.5384236695712103E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14">
         <f>D6-(D13*B6)</f>
-        <v>-1.9880992103214305E-3</v>
+        <v>-1.6348315528643374E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15">
         <f>1/D13</f>
-        <v>5754.2400000000007</v>
+        <v>6500.1600000000008</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16">
         <f>D14/D13</f>
-        <v>-11.439999999999991</v>
+        <v>-10.626666666666653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>